<commit_message>
se ajusta las respuestas del endpoint responde de forma intermedia falta naturalizar respuesta
</commit_message>
<xml_diff>
--- a/app/data/database/tourism_packages.xlsx
+++ b/app/data/database/tourism_packages.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer a10\Downloads\archivos prompt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3BA96C8-F452-4534-97EA-E23BEFB281E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2205F570-2B72-4719-A5A4-598125A61D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$62</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="440">
   <si>
     <t>id_package</t>
   </si>
@@ -1722,13 +1725,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1784,7 +1807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1840,7 +1863,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1896,7 +1919,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1952,7 +1975,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2008,7 +2031,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2064,7 +2087,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2120,7 +2143,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2176,7 +2199,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2232,7 +2255,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2288,7 +2311,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2344,7 +2367,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2400,7 +2423,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2456,7 +2479,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2512,7 +2535,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2568,7 +2591,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2624,7 +2647,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2680,7 +2703,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2736,7 +2759,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2792,7 +2815,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2848,7 +2871,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2897,8 +2920,14 @@
       <c r="P21" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q21" t="s">
+        <v>126</v>
+      </c>
+      <c r="R21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2954,7 +2983,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3010,7 +3039,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3066,7 +3095,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3122,7 +3151,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3178,7 +3207,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3234,7 +3263,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3290,7 +3319,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3346,7 +3375,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3402,7 +3431,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3458,7 +3487,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3514,7 +3543,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3570,7 +3599,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3626,7 +3655,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3682,7 +3711,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3738,7 +3767,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3794,7 +3823,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3850,7 +3879,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3906,7 +3935,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3962,7 +3991,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4018,7 +4047,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4074,7 +4103,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4130,7 +4159,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4186,7 +4215,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4242,7 +4271,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4298,7 +4327,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4354,7 +4383,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4410,7 +4439,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4466,7 +4495,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4522,7 +4551,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4578,7 +4607,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4634,7 +4663,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4690,7 +4719,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4746,7 +4775,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4802,7 +4831,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4858,7 +4887,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4914,7 +4943,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4970,7 +4999,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5026,7 +5055,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5082,7 +5111,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5138,7 +5167,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>

</xml_diff>